<commit_message>
change names variables and add script to include lat, long
</commit_message>
<xml_diff>
--- a/data/raw_data/dic_variables_serpam.xlsx
+++ b/data/raw_data/dic_variables_serpam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajpelu/SERPAM Dropbox/14_GBIF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D1E551-6B28-C847-A1D5-0587C5A85EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDF6690-0878-584C-B756-27086151A78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19800" xr2:uid="{B76C4D5A-98EF-774E-80E4-E1448A5E01AA}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{B76C4D5A-98EF-774E-80E4-E1448A5E01AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,9 +389,6 @@
     <t>V03</t>
   </si>
   <si>
-    <t xml:space="preserve">specific vegetation cover </t>
-  </si>
-  <si>
     <t xml:space="preserve">Étienne and Rigolot visual method </t>
   </si>
   <si>
@@ -557,9 +554,6 @@
     <t>lichen_cover</t>
   </si>
   <si>
-    <t>total specific cover</t>
-  </si>
-  <si>
     <t>total_specific_cover</t>
   </si>
   <si>
@@ -762,6 +756,12 @@
   </si>
   <si>
     <t>musk_percent_pq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specific plant cover </t>
+  </si>
+  <si>
+    <t>total specific plant cover</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EAC910-15BD-3E4A-A2E6-18290EA85459}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1157,7 +1157,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1174,7 +1174,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1453,7 +1453,7 @@
         <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
         <v>76</v>
@@ -1476,7 +1476,7 @@
         <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
         <v>82</v>
@@ -1585,22 +1585,22 @@
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>235</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H20" t="s">
         <v>108</v>
@@ -1611,22 +1611,22 @@
         <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>235</v>
       </c>
       <c r="C21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H21" t="s">
         <v>108</v>
@@ -1637,22 +1637,22 @@
         <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>235</v>
       </c>
       <c r="C22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H22" t="s">
         <v>108</v>
@@ -1660,25 +1660,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" t="s">
         <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H23" t="s">
         <v>108</v>
@@ -1686,25 +1686,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
         <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H24" t="s">
         <v>108</v>
@@ -1712,25 +1712,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" t="s">
         <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H25" t="s">
         <v>108</v>
@@ -1738,25 +1738,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
         <v>111</v>
       </c>
-      <c r="C26" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>112</v>
-      </c>
       <c r="F26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H26" t="s">
         <v>108</v>
@@ -1764,25 +1764,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H27" t="s">
         <v>108</v>
@@ -1790,25 +1790,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H28" t="s">
         <v>108</v>
@@ -1816,558 +1816,558 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
         <v>114</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" t="s">
         <v>116</v>
       </c>
-      <c r="E29" t="s">
-        <v>179</v>
-      </c>
-      <c r="F29" t="s">
-        <v>178</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>117</v>
-      </c>
-      <c r="H29" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
         <v>120</v>
       </c>
-      <c r="C30" t="s">
-        <v>121</v>
-      </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" t="s">
         <v>120</v>
       </c>
-      <c r="C31" t="s">
-        <v>121</v>
-      </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" t="s">
         <v>123</v>
       </c>
-      <c r="C32" t="s">
-        <v>124</v>
-      </c>
       <c r="D32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
         <v>123</v>
       </c>
-      <c r="C33" t="s">
-        <v>124</v>
-      </c>
       <c r="D33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G33" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
+        <v>183</v>
+      </c>
+      <c r="F34" t="s">
+        <v>171</v>
+      </c>
+      <c r="G34" t="s">
+        <v>221</v>
+      </c>
+      <c r="H34" t="s">
         <v>127</v>
-      </c>
-      <c r="E34" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" t="s">
-        <v>223</v>
-      </c>
-      <c r="H34" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" t="s">
         <v>126</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" t="s">
+        <v>223</v>
+      </c>
+      <c r="H35" t="s">
         <v>127</v>
-      </c>
-      <c r="E35" t="s">
-        <v>184</v>
-      </c>
-      <c r="F35" t="s">
-        <v>174</v>
-      </c>
-      <c r="G35" t="s">
-        <v>225</v>
-      </c>
-      <c r="H35" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36" t="s">
         <v>172</v>
       </c>
-      <c r="B36" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="G36" t="s">
+        <v>222</v>
+      </c>
+      <c r="H36" t="s">
         <v>127</v>
-      </c>
-      <c r="E36" t="s">
-        <v>183</v>
-      </c>
-      <c r="F36" t="s">
-        <v>174</v>
-      </c>
-      <c r="G36" t="s">
-        <v>224</v>
-      </c>
-      <c r="H36" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" t="s">
         <v>130</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>131</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" t="s">
+        <v>224</v>
+      </c>
+      <c r="H37" t="s">
         <v>132</v>
-      </c>
-      <c r="E37" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" t="s">
-        <v>173</v>
-      </c>
-      <c r="G37" t="s">
-        <v>226</v>
-      </c>
-      <c r="H37" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" t="s">
         <v>130</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>131</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G38" t="s">
+        <v>225</v>
+      </c>
+      <c r="H38" t="s">
         <v>132</v>
-      </c>
-      <c r="E38" t="s">
-        <v>187</v>
-      </c>
-      <c r="F38" t="s">
-        <v>174</v>
-      </c>
-      <c r="G38" t="s">
-        <v>227</v>
-      </c>
-      <c r="H38" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s">
         <v>130</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>131</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" t="s">
+        <v>226</v>
+      </c>
+      <c r="H39" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F39" t="s">
-        <v>174</v>
-      </c>
-      <c r="G39" t="s">
-        <v>228</v>
-      </c>
-      <c r="H39" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" t="s">
         <v>135</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>136</v>
       </c>
-      <c r="D40" t="s">
-        <v>137</v>
-      </c>
       <c r="E40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" t="s">
         <v>141</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" t="s">
+        <v>227</v>
+      </c>
+      <c r="H41" t="s">
         <v>142</v>
-      </c>
-      <c r="D41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" t="s">
-        <v>138</v>
-      </c>
-      <c r="F41" t="s">
-        <v>173</v>
-      </c>
-      <c r="G41" t="s">
-        <v>229</v>
-      </c>
-      <c r="H41" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" t="s">
         <v>141</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42" t="s">
+        <v>228</v>
+      </c>
+      <c r="H42" t="s">
         <v>142</v>
-      </c>
-      <c r="D42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s">
-        <v>175</v>
-      </c>
-      <c r="F42" t="s">
-        <v>174</v>
-      </c>
-      <c r="G42" t="s">
-        <v>230</v>
-      </c>
-      <c r="H42" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" t="s">
         <v>141</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" t="s">
+        <v>172</v>
+      </c>
+      <c r="G43" t="s">
+        <v>229</v>
+      </c>
+      <c r="H43" t="s">
         <v>142</v>
-      </c>
-      <c r="D43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" t="s">
-        <v>177</v>
-      </c>
-      <c r="F43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G43" t="s">
-        <v>231</v>
-      </c>
-      <c r="H43" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" t="s">
         <v>145</v>
       </c>
-      <c r="C44" t="s">
-        <v>146</v>
-      </c>
       <c r="D44" t="s">
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G44" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" t="s">
         <v>145</v>
       </c>
-      <c r="C45" t="s">
-        <v>146</v>
-      </c>
       <c r="D45" t="s">
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" t="s">
         <v>165</v>
       </c>
-      <c r="C46" t="s">
-        <v>166</v>
-      </c>
       <c r="D46" t="s">
         <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G46" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" t="s">
         <v>165</v>
       </c>
-      <c r="C47" t="s">
-        <v>166</v>
-      </c>
       <c r="D47" t="s">
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F47" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G47" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B48" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" t="s">
         <v>148</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>149</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>150</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
+        <v>171</v>
+      </c>
+      <c r="G48" t="s">
         <v>151</v>
-      </c>
-      <c r="F48" t="s">
-        <v>173</v>
-      </c>
-      <c r="G48" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
       </c>
       <c r="E49" t="s">
+        <v>153</v>
+      </c>
+      <c r="F49" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" t="s">
         <v>154</v>
-      </c>
-      <c r="F49" t="s">
-        <v>173</v>
-      </c>
-      <c r="G49" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" t="s">
         <v>157</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>153</v>
+      </c>
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+      <c r="G50" t="s">
         <v>158</v>
-      </c>
-      <c r="D50" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" t="s">
-        <v>154</v>
-      </c>
-      <c r="F50" t="s">
-        <v>173</v>
-      </c>
-      <c r="G50" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" t="s">
+        <v>204</v>
+      </c>
+      <c r="C51" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" t="s">
         <v>205</v>
       </c>
-      <c r="B51" t="s">
+      <c r="E51" t="s">
         <v>206</v>
       </c>
-      <c r="C51" t="s">
-        <v>206</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
+        <v>171</v>
+      </c>
+      <c r="G51" t="s">
+        <v>204</v>
+      </c>
+      <c r="H51" t="s">
         <v>207</v>
-      </c>
-      <c r="E51" t="s">
-        <v>208</v>
-      </c>
-      <c r="F51" t="s">
-        <v>173</v>
-      </c>
-      <c r="G51" t="s">
-        <v>206</v>
-      </c>
-      <c r="H51" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>